<commit_message>
small edits to documentation
</commit_message>
<xml_diff>
--- a/test-files/test-file-documentation.xlsx
+++ b/test-files/test-file-documentation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8000" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13880" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="gene-name-modifications" sheetId="1" r:id="rId1"/>
@@ -321,13 +321,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,7 +830,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -847,232 +848,232 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="A9" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="A10" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" t="s">
+      <c r="A21" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" t="s">
+      <c r="A22" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" t="s">
+      <c r="A23" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" t="s">
+      <c r="A24" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" t="s">
+      <c r="A25" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" t="s">
+      <c r="A26" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" t="s">
+      <c r="A27" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" t="s">
+      <c r="A28" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" t="s">
+      <c r="A30" s="6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" t="s">
+      <c r="A31" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" t="s">
+      <c r="A32" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" t="s">
+      <c r="A33" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" t="s">
+      <c r="A34" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" t="s">
+      <c r="A35" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" t="s">
+      <c r="A36" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" t="s">
+      <c r="A37" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" t="s">
+      <c r="A38" s="6" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" t="s">
+      <c r="A39" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" t="s">
+      <c r="A40" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" t="s">
+      <c r="A41" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" t="s">
+      <c r="A42" s="6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" t="s">
+      <c r="A43" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" t="s">
+      <c r="A44" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" t="s">
+      <c r="A45" s="6" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" t="s">
+      <c r="A46" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" t="s">
+      <c r="A47" s="6" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>